<commit_message>
added search module, next to work on adding item to cart
</commit_message>
<xml_diff>
--- a/excelfiles/input.xlsx
+++ b/excelfiles/input.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>mypassword@</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t>avengers</t>
+  </si>
+  <si>
+    <t>iron man</t>
+  </si>
+  <si>
+    <t>hulk</t>
   </si>
 </sst>
 </file>
@@ -361,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,6 +388,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>

</xml_diff>